<commit_message>
changed Tank_Control3.py for testing. other changes are negligible
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -379,37 +379,102 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>-363.73</v>
+        <v>-142.35</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>-468.36</v>
+        <v>-97.52000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>-714.36</v>
+        <v>-307.34</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>-774</v>
+        <v>-603.36</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>-774</v>
+        <v>-603.36</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>-774</v>
+        <v>-603.36</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>-774</v>
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>-603.36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>-603.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>